<commit_message>
update test.xlsx và qlproduct 27/02 - tan
</commit_message>
<xml_diff>
--- a/src/test/resources/TestCartData.xlsx
+++ b/src/test/resources/TestCartData.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
   <si>
     <t>Success</t>
   </si>
@@ -125,6 +125,54 @@
 Command: [859fd7f9870f95acc9b79de45eb47519, findElement {using=xpath, value=//div[contains(@class,'product-card')][.//a[contains(normalize-space(.),'New Balance 550')]]//button[contains(@class,'btn-dark') or contains(normalize-space(.),'MUA')]}]
 Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 145.0.7632.111, chrome: {chromedriverVersion: 145.0.7632.117 (de4e5d6e13b..., userDataDir: C:\Users\pc\AppData\Local\T...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:53884}, goog:processID: 19948, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:53884/devtoo..., se:cdpVersion: 145.0.7632.111, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
 Session ID: 859fd7f9870f95acc9b79de45eb47519</t>
+  </si>
+  <si>
+    <t>Lỗi: Expected condition failed: waiting for element to be clickable: By.xpath: //div[contains(@class,'product-card')][.//a[contains(normalize-space(.),'Vans Old Skool')]]//button[contains(@class,'btn-dark') or contains(normalize-space(.),'MUA')] (tried for 15 second(s) with 500 milliseconds interval)
+Build info: version: '4.14.1', revision: '03f8ede370'
+System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '17.0.10'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 145.0.7632.111, chrome: {chromedriverVersion: 145.0.7632.117 (de4e5d6e13b..., userDataDir: C:\Users\tanng\AppData\Loca...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:63620}, goog:processID: 16052, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:63620/devtoo..., se:cdpVersion: 145.0.7632.111, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 0015102cfb92e088fda97195c3648cd3</t>
+  </si>
+  <si>
+    <t>Lỗi: Expected condition failed: waiting for element to be clickable: By.xpath: //div[contains(@class,'product-card')][.//a[contains(normalize-space(.),'Puma Suede Classic')]]//button[contains(@class,'btn-dark') or contains(normalize-space(.),'MUA')] (tried for 15 second(s) with 500 milliseconds interval)
+Build info: version: '4.14.1', revision: '03f8ede370'
+System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '17.0.10'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 145.0.7632.111, chrome: {chromedriverVersion: 145.0.7632.117 (de4e5d6e13b..., userDataDir: C:\Users\tanng\AppData\Loca...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:63620}, goog:processID: 16052, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:63620/devtoo..., se:cdpVersion: 145.0.7632.111, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 0015102cfb92e088fda97195c3648cd3</t>
+  </si>
+  <si>
+    <t>Lỗi: Expected condition failed: waiting for element to be clickable: By.xpath: //div[contains(@class,'product-card')][.//a[contains(normalize-space(.),'Converse Chuck 70')]]//button[contains(@class,'btn-dark') or contains(normalize-space(.),'MUA')] (tried for 15 second(s) with 500 milliseconds interval)
+Build info: version: '4.14.1', revision: '03f8ede370'
+System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '17.0.10'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 145.0.7632.111, chrome: {chromedriverVersion: 145.0.7632.117 (de4e5d6e13b..., userDataDir: C:\Users\tanng\AppData\Loca...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:63620}, goog:processID: 16052, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:63620/devtoo..., se:cdpVersion: 145.0.7632.111, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 0015102cfb92e088fda97195c3648cd3</t>
+  </si>
+  <si>
+    <t>Lỗi: Expected condition failed: waiting for element to be clickable: By.xpath: //div[contains(@class,'product-card')][.//a[contains(normalize-space(.),'Nike Air Force 1')]]//button[contains(@class,'btn-dark') or contains(normalize-space(.),'MUA')] (tried for 15 second(s) with 500 milliseconds interval)
+Build info: version: '4.14.1', revision: '03f8ede370'
+System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '17.0.10'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 145.0.7632.111, chrome: {chromedriverVersion: 145.0.7632.117 (de4e5d6e13b..., userDataDir: C:\Users\tanng\AppData\Loca...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:63620}, goog:processID: 16052, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:63620/devtoo..., se:cdpVersion: 145.0.7632.111, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 0015102cfb92e088fda97195c3648cd3</t>
+  </si>
+  <si>
+    <t>Lỗi: Expected condition failed: waiting for element to be clickable: By.xpath: //div[contains(@class,'product-card')][.//a[contains(normalize-space(.),'New Balance 550')]]//button[contains(@class,'btn-dark') or contains(normalize-space(.),'MUA')] (tried for 15 second(s) with 500 milliseconds interval)
+Build info: version: '4.14.1', revision: '03f8ede370'
+System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '17.0.10'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 145.0.7632.111, chrome: {chromedriverVersion: 145.0.7632.117 (de4e5d6e13b..., userDataDir: C:\Users\tanng\AppData\Loca...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:63620}, goog:processID: 16052, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:63620/devtoo..., se:cdpVersion: 145.0.7632.111, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 0015102cfb92e088fda97195c3648cd3</t>
+  </si>
+  <si>
+    <t>Lỗi: Expected condition failed: waiting for element to be clickable: By.xpath: //div[contains(@class,'product-card')][.//a[contains(normalize-space(.),'Adidas Superstar')]]//button[contains(@class,'btn-dark') or contains(normalize-space(.),'MUA')] (tried for 15 second(s) with 500 milliseconds interval)
+Build info: version: '4.14.1', revision: '03f8ede370'
+System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '17.0.10'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 145.0.7632.111, chrome: {chromedriverVersion: 145.0.7632.117 (de4e5d6e13b..., userDataDir: C:\Users\tanng\AppData\Loca...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:63620}, goog:processID: 16052, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:63620/devtoo..., se:cdpVersion: 145.0.7632.111, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 0015102cfb92e088fda97195c3648cd3</t>
   </si>
 </sst>
 </file>
@@ -483,7 +531,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F2" t="s" s="0">
         <v>16</v>
@@ -503,7 +551,7 @@
         <v>2</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F3" t="s" s="0">
         <v>16</v>
@@ -523,7 +571,7 @@
         <v>3</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s" s="0">
         <v>16</v>
@@ -543,7 +591,7 @@
         <v>4</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="F5" t="s" s="0">
         <v>16</v>
@@ -563,7 +611,7 @@
         <v>5</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="F6" t="s" s="0">
         <v>16</v>
@@ -583,7 +631,7 @@
         <v>6</v>
       </c>
       <c r="E7" t="s" s="0">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="F7" t="s" s="0">
         <v>16</v>

</xml_diff>